<commit_message>
Fix adding multiple localized values Set min inflate ratio
</commit_message>
<xml_diff>
--- a/src/test/resources/importapi/excel/excel_export.xlsx
+++ b/src/test/resources/importapi/excel/excel_export.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kalle.kyttala/DVV/build.master/yti-terminology-api/src/test/resources/importapi/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29600E76-55E6-F941-976E-BC532AC31C9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D51751F3-A8E3-E745-B96D-8F5F15CD87F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Terminology details" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="128">
   <si>
     <t>terminological-vocabulary-0</t>
   </si>
@@ -284,9 +284,6 @@
     <t>http://uri.suomi.fi/terminology/erergerg/concept-0</t>
   </si>
   <si>
-    <t>Definition FI</t>
-  </si>
-  <si>
     <t>Definition EN</t>
   </si>
   <si>
@@ -308,9 +305,6 @@
     <t>Source</t>
   </si>
   <si>
-    <t>Note EN</t>
-  </si>
-  <si>
     <t>Note FI</t>
   </si>
   <si>
@@ -404,10 +398,16 @@
     <t>http://uri.suomi.fi/terminology/testdev/term-1</t>
   </si>
   <si>
-    <t>test term</t>
-  </si>
-  <si>
-    <t>test term  en</t>
+    <t>Definition FI 2</t>
+  </si>
+  <si>
+    <t>Definition FI 1</t>
+  </si>
+  <si>
+    <t>Note EN 2</t>
+  </si>
+  <si>
+    <t>Note EN 1</t>
   </si>
 </sst>
 </file>
@@ -455,7 +455,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -470,10 +470,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -791,7 +793,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
@@ -843,10 +845,10 @@
       <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="L1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="12"/>
+      <c r="M1" s="13"/>
       <c r="N1" t="s">
         <v>11</v>
       </c>
@@ -865,10 +867,10 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -877,7 +879,7 @@
         <v>57</v>
       </c>
       <c r="E2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F2" t="s">
         <v>62</v>
@@ -886,7 +888,7 @@
         <v>3</v>
       </c>
       <c r="H2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -953,10 +955,10 @@
       <c r="D1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="13"/>
+      <c r="F1" s="14"/>
       <c r="G1" t="s">
         <v>12</v>
       </c>
@@ -1010,10 +1012,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AH2"/>
+  <dimension ref="A1:AK2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1024,32 +1026,38 @@
     <col min="5" max="5" width="36.5" customWidth="1"/>
     <col min="6" max="6" width="25.1640625" customWidth="1"/>
     <col min="7" max="7" width="15.33203125" customWidth="1"/>
-    <col min="8" max="8" width="15.83203125" style="7" customWidth="1"/>
-    <col min="9" max="13" width="8.83203125" style="7"/>
-    <col min="14" max="14" width="11.83203125" style="7" customWidth="1"/>
-    <col min="15" max="15" width="8.83203125" style="7"/>
-    <col min="16" max="16" width="16.1640625" style="7" customWidth="1"/>
-    <col min="17" max="17" width="22.6640625" style="7" customWidth="1"/>
-    <col min="21" max="21" width="38.33203125" customWidth="1"/>
-    <col min="22" max="22" width="18.1640625" customWidth="1"/>
-    <col min="24" max="24" width="43.5" customWidth="1"/>
-    <col min="27" max="27" width="24.6640625" customWidth="1"/>
-    <col min="28" max="28" width="33.33203125" customWidth="1"/>
-    <col min="30" max="30" width="25" customWidth="1"/>
-    <col min="33" max="33" width="56.6640625" customWidth="1"/>
+    <col min="8" max="8" width="23.1640625" style="7" customWidth="1"/>
+    <col min="9" max="10" width="23.1640625" style="12" customWidth="1"/>
+    <col min="11" max="11" width="13.5" style="7" customWidth="1"/>
+    <col min="12" max="12" width="8.83203125" style="7"/>
+    <col min="13" max="13" width="12" style="12" customWidth="1"/>
+    <col min="14" max="14" width="13.1640625" style="7" customWidth="1"/>
+    <col min="15" max="15" width="20.1640625" style="7" customWidth="1"/>
+    <col min="16" max="16" width="8.83203125" style="7"/>
+    <col min="17" max="17" width="11.83203125" style="7" customWidth="1"/>
+    <col min="18" max="18" width="8.83203125" style="7"/>
+    <col min="19" max="19" width="16.1640625" style="7" customWidth="1"/>
+    <col min="20" max="20" width="22.6640625" style="7" customWidth="1"/>
+    <col min="24" max="24" width="38.33203125" customWidth="1"/>
+    <col min="25" max="25" width="18.1640625" customWidth="1"/>
+    <col min="27" max="27" width="43.5" customWidth="1"/>
+    <col min="30" max="30" width="24.6640625" customWidth="1"/>
+    <col min="31" max="31" width="33.33203125" customWidth="1"/>
+    <col min="33" max="33" width="25" customWidth="1"/>
+    <col min="36" max="36" width="56.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>58</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="13"/>
+      <c r="D1" s="14"/>
       <c r="E1" t="s">
         <v>26</v>
       </c>
@@ -1059,161 +1067,172 @@
       <c r="G1" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="M1" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="N1" s="15"/>
+      <c r="O1" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="P1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="Q1" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="R1" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="S1" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="T1" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="R1" t="s">
+      <c r="U1" t="s">
         <v>9</v>
       </c>
-      <c r="S1" t="s">
+      <c r="V1" t="s">
         <v>34</v>
       </c>
-      <c r="T1" t="s">
+      <c r="W1" t="s">
         <v>35</v>
       </c>
-      <c r="U1" t="s">
+      <c r="X1" t="s">
         <v>36</v>
       </c>
-      <c r="V1" s="13" t="s">
+      <c r="Y1" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="W1" s="13"/>
-      <c r="X1" t="s">
+      <c r="Z1" s="14"/>
+      <c r="AA1" t="s">
         <v>38</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AB1" t="s">
         <v>39</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AC1" t="s">
         <v>40</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AD1" t="s">
         <v>41</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AE1" t="s">
         <v>42</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AF1" t="s">
         <v>43</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AG1" t="s">
         <v>44</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AH1" t="s">
         <v>12</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AI1" t="s">
         <v>13</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AJ1" t="s">
         <v>15</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AK1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s">
         <v>22</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H2" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="K2" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="L2" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="O2" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="P2" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q2" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="R2" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="S2" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="T2" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="K2" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="O2" s="7" t="s">
+      <c r="U2" t="s">
+        <v>8</v>
+      </c>
+      <c r="V2" t="s">
         <v>91</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="W2" t="s">
+        <v>92</v>
+      </c>
+      <c r="X2" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="Q2" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="R2" t="s">
-        <v>8</v>
-      </c>
-      <c r="S2" t="s">
-        <v>92</v>
-      </c>
-      <c r="T2" t="s">
-        <v>93</v>
-      </c>
-      <c r="U2" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="X2" s="7" t="s">
+      <c r="AA2" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="AE2" s="5">
+      <c r="AH2" s="5">
         <v>44320.497349537036</v>
       </c>
-      <c r="AF2" s="6">
+      <c r="AI2" s="6">
         <v>44320.497349537036</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AJ2" t="s">
         <v>45</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AK2" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="C1:D1"/>
-    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="Y1:Z1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="M1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1222,211 +1241,195 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:T3"/>
+  <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="13.33203125" style="7" customWidth="1"/>
-    <col min="4" max="4" width="13.83203125" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" customWidth="1"/>
-    <col min="15" max="15" width="16.5" customWidth="1"/>
-    <col min="16" max="16" width="16.1640625" customWidth="1"/>
-    <col min="19" max="19" width="47.1640625" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" customWidth="1"/>
+    <col min="14" max="14" width="16.5" customWidth="1"/>
+    <col min="15" max="15" width="16.1640625" customWidth="1"/>
+    <col min="18" max="18" width="47.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>76</v>
+      <c r="B1" t="s">
+        <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K1" t="s">
+        <v>52</v>
+      </c>
+      <c r="L1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" t="s">
+        <v>53</v>
+      </c>
+      <c r="N1" t="s">
+        <v>54</v>
+      </c>
+      <c r="O1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H2" t="s">
+        <v>67</v>
+      </c>
+      <c r="I2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J2" t="s">
+        <v>69</v>
+      </c>
+      <c r="K2" t="s">
+        <v>70</v>
+      </c>
+      <c r="L2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M2">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I1" t="s">
-        <v>49</v>
-      </c>
-      <c r="J1" t="s">
-        <v>50</v>
-      </c>
-      <c r="K1" t="s">
-        <v>51</v>
-      </c>
-      <c r="L1" t="s">
-        <v>52</v>
-      </c>
-      <c r="M1" t="s">
-        <v>31</v>
-      </c>
-      <c r="N1" t="s">
-        <v>53</v>
-      </c>
-      <c r="O1" t="s">
-        <v>54</v>
-      </c>
-      <c r="P1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>32</v>
-      </c>
-      <c r="R1" t="s">
-        <v>9</v>
-      </c>
-      <c r="S1" t="s">
-        <v>15</v>
-      </c>
-      <c r="T1" t="s">
-        <v>17</v>
+      <c r="N2" t="s">
+        <v>74</v>
+      </c>
+      <c r="O2" t="s">
+        <v>73</v>
+      </c>
+      <c r="P2" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>8</v>
+      </c>
+      <c r="R2" t="s">
+        <v>55</v>
+      </c>
+      <c r="S2" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="C2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" t="s">
-        <v>119</v>
-      </c>
-      <c r="E2" t="s">
-        <v>120</v>
-      </c>
-      <c r="F2" t="s">
+    <row r="3" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="G2" t="s">
+      <c r="F3" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="H2" t="s">
+      <c r="G3" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="I2" t="s">
+      <c r="H3" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="J2" t="s">
+      <c r="I3" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="K2" t="s">
+      <c r="J3" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="L2" t="s">
+      <c r="K3" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="M2" t="s">
+      <c r="L3" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="N2">
+      <c r="M3" s="8">
         <v>1</v>
       </c>
-      <c r="O2" t="s">
+      <c r="N3" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="P2" t="s">
+      <c r="O3" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="P3" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="R2" t="s">
+      <c r="Q3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="S2" t="s">
-        <v>55</v>
-      </c>
-      <c r="T2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="N3" s="8">
-        <v>1</v>
-      </c>
-      <c r="O3" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="P3" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q3" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="R3" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="S3" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="T3" s="8" t="s">
+      <c r="R3" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="S3" s="8" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="S3" r:id="rId1" xr:uid="{0A389625-E6B0-B547-B63A-58530F93ED7B}"/>
+    <hyperlink ref="R3" r:id="rId1" xr:uid="{0A389625-E6B0-B547-B63A-58530F93ED7B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1462,22 +1465,22 @@
         <v>1</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>76</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G1" s="8" t="s">
         <v>2</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="I1" s="8" t="s">
         <v>15</v>
@@ -1488,31 +1491,31 @@
     </row>
     <row r="2" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="C2" s="8" t="s">
+      <c r="F2" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="E2" s="8" t="s">
+      <c r="G2" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="F2" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="H2" s="8" t="s">
+      <c r="I2" s="10" t="s">
         <v>110</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>112</v>
       </c>
       <c r="J2" s="8" t="s">
         <v>16</v>
@@ -1520,31 +1523,31 @@
     </row>
     <row r="3" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B3" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="G3" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="H3" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="I3" s="10" t="s">
         <v>114</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>116</v>
       </c>
       <c r="J3" s="8" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
Empty identifier and uri for placeholder terms remove placeholder from the map after handling
</commit_message>
<xml_diff>
--- a/src/test/resources/importapi/excel/excel_export.xlsx
+++ b/src/test/resources/importapi/excel/excel_export.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kalle.kyttala/DVV/build.master/yti-terminology-api/src/test/resources/importapi/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D51751F3-A8E3-E745-B96D-8F5F15CD87F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2592A802-6AF0-0B48-B640-585A8DDDAA08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Terminology details" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="130">
   <si>
     <t>terminological-vocabulary-0</t>
   </si>
@@ -408,6 +408,12 @@
   </si>
   <si>
     <t>Note EN 1</t>
+  </si>
+  <si>
+    <t>c73c8ed4-ce6e-4660-b42c-e3908a788021</t>
+  </si>
+  <si>
+    <t>term placeholder</t>
   </si>
 </sst>
 </file>
@@ -455,7 +461,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -469,6 +475,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -845,10 +852,10 @@
       <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="L1" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="13"/>
+      <c r="M1" s="14"/>
       <c r="N1" t="s">
         <v>11</v>
       </c>
@@ -955,10 +962,10 @@
       <c r="D1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="14"/>
+      <c r="F1" s="15"/>
       <c r="G1" t="s">
         <v>12</v>
       </c>
@@ -1012,10 +1019,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AK2"/>
+  <dimension ref="A1:AL2"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1023,134 +1030,136 @@
     <col min="2" max="2" width="11.6640625" customWidth="1"/>
     <col min="3" max="3" width="15.83203125" customWidth="1"/>
     <col min="4" max="4" width="22.83203125" customWidth="1"/>
-    <col min="5" max="5" width="36.5" customWidth="1"/>
-    <col min="6" max="6" width="25.1640625" customWidth="1"/>
-    <col min="7" max="7" width="15.33203125" customWidth="1"/>
-    <col min="8" max="8" width="23.1640625" style="7" customWidth="1"/>
-    <col min="9" max="10" width="23.1640625" style="12" customWidth="1"/>
-    <col min="11" max="11" width="13.5" style="7" customWidth="1"/>
-    <col min="12" max="12" width="8.83203125" style="7"/>
-    <col min="13" max="13" width="12" style="12" customWidth="1"/>
-    <col min="14" max="14" width="13.1640625" style="7" customWidth="1"/>
-    <col min="15" max="15" width="20.1640625" style="7" customWidth="1"/>
-    <col min="16" max="16" width="8.83203125" style="7"/>
-    <col min="17" max="17" width="11.83203125" style="7" customWidth="1"/>
-    <col min="18" max="18" width="8.83203125" style="7"/>
-    <col min="19" max="19" width="16.1640625" style="7" customWidth="1"/>
-    <col min="20" max="20" width="22.6640625" style="7" customWidth="1"/>
-    <col min="24" max="24" width="38.33203125" customWidth="1"/>
-    <col min="25" max="25" width="18.1640625" customWidth="1"/>
-    <col min="27" max="27" width="43.5" customWidth="1"/>
-    <col min="30" max="30" width="24.6640625" customWidth="1"/>
-    <col min="31" max="31" width="33.33203125" customWidth="1"/>
-    <col min="33" max="33" width="25" customWidth="1"/>
-    <col min="36" max="36" width="56.6640625" customWidth="1"/>
+    <col min="5" max="5" width="22.83203125" style="13" customWidth="1"/>
+    <col min="6" max="6" width="36.5" customWidth="1"/>
+    <col min="7" max="7" width="25.1640625" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" customWidth="1"/>
+    <col min="9" max="9" width="23.1640625" style="7" customWidth="1"/>
+    <col min="10" max="11" width="23.1640625" style="12" customWidth="1"/>
+    <col min="12" max="12" width="13.5" style="7" customWidth="1"/>
+    <col min="13" max="13" width="8.83203125" style="7"/>
+    <col min="14" max="14" width="12" style="12" customWidth="1"/>
+    <col min="15" max="15" width="13.1640625" style="7" customWidth="1"/>
+    <col min="16" max="16" width="20.1640625" style="7" customWidth="1"/>
+    <col min="17" max="17" width="8.83203125" style="7"/>
+    <col min="18" max="18" width="11.83203125" style="7" customWidth="1"/>
+    <col min="19" max="19" width="8.83203125" style="7"/>
+    <col min="20" max="20" width="16.1640625" style="7" customWidth="1"/>
+    <col min="21" max="21" width="22.6640625" style="7" customWidth="1"/>
+    <col min="25" max="25" width="38.33203125" customWidth="1"/>
+    <col min="26" max="26" width="18.1640625" customWidth="1"/>
+    <col min="28" max="28" width="43.5" customWidth="1"/>
+    <col min="31" max="31" width="24.6640625" customWidth="1"/>
+    <col min="32" max="32" width="33.33203125" customWidth="1"/>
+    <col min="34" max="34" width="25" customWidth="1"/>
+    <col min="37" max="37" width="56.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>58</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="14"/>
-      <c r="E1" t="s">
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" t="s">
         <v>26</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>27</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="I1" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="7" t="s">
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="M1" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="M1" s="15" t="s">
+      <c r="N1" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="N1" s="15"/>
-      <c r="O1" s="7" t="s">
+      <c r="O1" s="16"/>
+      <c r="P1" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="Q1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="R1" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="S1" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="T1" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="U1" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>9</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>34</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>35</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>36</v>
       </c>
-      <c r="Y1" s="14" t="s">
+      <c r="Z1" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="Z1" s="14"/>
-      <c r="AA1" t="s">
+      <c r="AA1" s="15"/>
+      <c r="AB1" t="s">
         <v>38</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>39</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>40</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>41</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>42</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>43</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>44</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>12</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>13</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>15</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>98</v>
       </c>
@@ -1160,79 +1169,82 @@
       <c r="C2" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="F2" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="I2" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="J2" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="L2" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="M2" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="N2" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="O2" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="P2" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="P2" s="7" t="s">
+      <c r="Q2" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="Q2" s="7" t="s">
+      <c r="R2" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="R2" s="7" t="s">
+      <c r="S2" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="S2" s="9" t="s">
+      <c r="T2" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="T2" s="7" t="s">
+      <c r="U2" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>8</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>91</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>92</v>
       </c>
-      <c r="X2" s="7" t="s">
+      <c r="Y2" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="AA2" s="7" t="s">
+      <c r="AB2" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="AH2" s="5">
+      <c r="AI2" s="5">
         <v>44320.497349537036</v>
       </c>
-      <c r="AI2" s="6">
+      <c r="AJ2" s="6">
         <v>44320.497349537036</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AK2" t="s">
         <v>45</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="AL2" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="Y1:Z1"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="Z1:AA1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="C1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1241,22 +1253,24 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:S3"/>
+  <dimension ref="A1:T4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="34.83203125" customWidth="1"/>
     <col min="3" max="3" width="13.83203125" customWidth="1"/>
     <col min="4" max="4" width="13.6640625" customWidth="1"/>
-    <col min="14" max="14" width="16.5" customWidth="1"/>
-    <col min="15" max="15" width="16.1640625" customWidth="1"/>
-    <col min="18" max="18" width="47.1640625" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" style="13" customWidth="1"/>
+    <col min="15" max="15" width="16.5" customWidth="1"/>
+    <col min="16" max="16" width="16.1640625" customWidth="1"/>
+    <col min="19" max="19" width="47.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>58</v>
       </c>
@@ -1269,53 +1283,56 @@
       <c r="D1" t="s">
         <v>46</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" t="s">
         <v>35</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>47</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>48</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>49</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>50</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>51</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>52</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>31</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>53</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>54</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>33</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>32</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>9</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>15</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>97</v>
       </c>
@@ -1325,53 +1342,53 @@
       <c r="C2" t="s">
         <v>117</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>64</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>65</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>66</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>67</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>68</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>69</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>70</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>71</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>1</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>74</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>73</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>75</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>8</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>55</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>116</v>
       </c>
@@ -1381,55 +1398,71 @@
       <c r="D3" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="13"/>
+      <c r="F3" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="G3" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="H3" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="I3" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="J3" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="K3" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="L3" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="L3" s="8" t="s">
+      <c r="M3" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="M3" s="8">
+      <c r="N3" s="8">
         <v>1</v>
       </c>
-      <c r="N3" s="8" t="s">
+      <c r="O3" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="O3" s="8" t="s">
+      <c r="P3" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="P3" s="8" t="s">
+      <c r="Q3" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="Q3" s="8" t="s">
+      <c r="R3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="R3" s="10" t="s">
+      <c r="S3" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="S3" s="8" t="s">
+      <c r="T3" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="R4" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="S4" s="10"/>
+      <c r="T4" s="13" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="R3" r:id="rId1" xr:uid="{0A389625-E6B0-B547-B63A-58530F93ED7B}"/>
+    <hyperlink ref="S3" r:id="rId1" xr:uid="{0A389625-E6B0-B547-B63A-58530F93ED7B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>